<commit_message>
add openspec to project, emails to rrhh sent
</commit_message>
<xml_diff>
--- a/rrhh_listado_correos.xlsx
+++ b/rrhh_listado_correos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlospsc/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlospsc/Desktop/envio-correos-comunicado-alexia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C1AAEA9-366A-2149-8175-0258ECB3A8E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0ACA649-748D-3747-8AD5-04FF8B93E108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1880" windowWidth="28040" windowHeight="17180" xr2:uid="{E6F17C43-E281-6E48-903D-E5A35B3B30A6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
   <si>
     <t>acarrascoc@einex.cl</t>
   </si>
@@ -429,9 +429,6 @@
   </si>
   <si>
     <t>yessenia.tobar@andessalud.cl</t>
-  </si>
-  <si>
-    <t>Nombre</t>
   </si>
   <si>
     <t>Correo</t>
@@ -814,674 +811,671 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDD23B51-89C1-8543-94AD-498801E064CA}">
-  <dimension ref="A1:B132"/>
+  <dimension ref="A1:A132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>131</v>
       </c>
-      <c r="B1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="1" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B34" s="1" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B35" s="1" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B36" s="1" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B39" s="1" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B40" s="1" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B41" s="1" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B42" s="1" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B44" s="1" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B45" s="1" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B46" s="1" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B47" s="1" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B48" s="1" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B49" s="1" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B50" s="1" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B51" s="1" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B52" s="1" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B53" s="1" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B54" s="1" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B55" s="1" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B56" s="1" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B57" s="1" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B58" s="1" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B59" s="1" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B60" s="1" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B61" s="1" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B62" s="1" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B63" s="1" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B64" s="1" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B65" s="1" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B66" s="1" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B67" s="1" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B68" s="1" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B69" s="1" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B70" s="1" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B71" s="1" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B72" s="1" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B73" s="1" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B74" s="1" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B75" s="1" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B76" s="1" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B77" s="1" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B78" s="1" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B79" s="1" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B80" s="1" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B81" s="1" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B82" s="1" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B83" s="1" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B84" s="1" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B85" s="1" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B86" s="1" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B87" s="1" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B88" s="1" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B89" s="1" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B90" s="1" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B91" s="1" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B92" s="1" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B93" s="1" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B94" s="1" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B95" s="1" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B96" s="1" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B97" s="1" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B98" s="1" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B99" s="1" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B100" s="1" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B101" s="1" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B102" s="1" t="s">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B103" s="1" t="s">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B104" s="1" t="s">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B105" s="1" t="s">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B106" s="1" t="s">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B107" s="1" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B108" s="1" t="s">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B109" s="1" t="s">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B110" s="1" t="s">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B111" s="1" t="s">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B112" s="1" t="s">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B113" s="1" t="s">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B114" s="1" t="s">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B115" s="1" t="s">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B116" s="1" t="s">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B117" s="1" t="s">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B118" s="1" t="s">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B119" s="1" t="s">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B120" s="1" t="s">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B121" s="1" t="s">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B122" s="1" t="s">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B123" s="1" t="s">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B124" s="1" t="s">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B125" s="1" t="s">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B126" s="1" t="s">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B127" s="1" t="s">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B128" s="1" t="s">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B129" s="1" t="s">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B130" s="1" t="s">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B131" s="1" t="s">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B132" s="1" t="s">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="s">
         <v>130</v>
       </c>
     </row>

</xml_diff>